<commit_message>
Update Methodology Summary_Andes 12.16.xlsx
</commit_message>
<xml_diff>
--- a/Inputs/Methodology Summary_Andes 12.16.xlsx
+++ b/Inputs/Methodology Summary_Andes 12.16.xlsx
@@ -3608,8 +3608,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e06ed64c304ede68fbf146ec0a2cc6f3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d2f6e290bc3f24965bc54ef07ecce9ef" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b17f52af6646b5583120346a68295973">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95a1201d1da507c70fe2596948b34472" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
     <xsd:import namespace="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
     <xsd:element name="properties">
@@ -3643,7 +3643,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="69276225-f05c-44c5-92dc-c999460a4149" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -3662,7 +3662,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -3694,7 +3694,7 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c40d4899-0986-466d-9443-4d7b8518a0f2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c40d4899-0986-466d-9443-4d7b8518a0f2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -3760,8 +3760,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -3876,20 +3876,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2EE7562-E997-4216-A724-18548DB05370}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC5BE481-FDE8-4633-AC9A-F5EDCFDDF5DB}"/>
 </file>
</xml_diff>